<commit_message>
Progress on chlorophyll data
</commit_message>
<xml_diff>
--- a/ohio2016/inputData/J. Beaulieu Chlorophyll 2016/Beaulieu 07272016.xlsx
+++ b/ohio2016/inputData/J. Beaulieu Chlorophyll 2016/Beaulieu 07272016.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kwyatt\Desktop\J. Beaulieu Chlorophyll 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JBEAULIE\GitRepository\mulitResSurvey\ohio2016\inputData\J. Beaulieu Chlorophyll 2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15180" windowHeight="8835"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="15180" windowHeight="8832"/>
   </bookViews>
   <sheets>
     <sheet name="CHL-A" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -295,6 +295,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -330,6 +347,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -482,38 +516,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -533,12 +565,12 @@
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -558,7 +590,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -577,13 +609,8 @@
       <c r="F9" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -602,10 +629,8 @@
       <c r="F10" s="3">
         <v>0.19</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -624,9 +649,8 @@
       <c r="F11">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -646,7 +670,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -666,7 +690,7 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -686,7 +710,7 @@
         <v>2.0199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -706,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -726,7 +750,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -746,7 +770,7 @@
         <v>5.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -766,7 +790,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -786,7 +810,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -806,7 +830,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -826,7 +850,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -846,7 +870,7 @@
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -866,7 +890,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -886,7 +910,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -906,7 +930,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -926,7 +950,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -946,7 +970,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -966,7 +990,7 @@
         <v>2.3E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -986,7 +1010,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1006,7 +1030,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1026,7 +1050,7 @@
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -1046,7 +1070,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -1066,7 +1090,7 @@
         <v>2.8299999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
@@ -1086,7 +1110,7 @@
         <v>2.87E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1106,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1126,7 +1150,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1146,7 +1170,7 @@
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -1166,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -1186,7 +1210,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -1206,7 +1230,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -1225,13 +1249,8 @@
       <c r="F41">
         <v>1.09E-2</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -1250,13 +1269,8 @@
       <c r="F42">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -1275,13 +1289,8 @@
       <c r="F43">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -1301,7 +1310,7 @@
         <v>9.2399999999999996E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Refinements to chl a data work up
</commit_message>
<xml_diff>
--- a/ohio2016/inputData/J. Beaulieu Chlorophyll 2016/Beaulieu 07272016.xlsx
+++ b/ohio2016/inputData/J. Beaulieu Chlorophyll 2016/Beaulieu 07272016.xlsx
@@ -126,18 +126,6 @@
     <t>BE2</t>
   </si>
   <si>
-    <t>07262016.WKA.SU01.3.1.UNK</t>
-  </si>
-  <si>
-    <t>07262016.WKA.SU01.3.1.UNK-A</t>
-  </si>
-  <si>
-    <t>07262016.WKA.SU01.15.UNK</t>
-  </si>
-  <si>
-    <t>07262016.WKA.SU01.15.UNK-A</t>
-  </si>
-  <si>
     <t>07212016.AVL.S06.0.1.UNK</t>
   </si>
   <si>
@@ -154,6 +142,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Date: 08/24/2016</t>
+  </si>
+  <si>
+    <t>07262016.WKA.SU-30.3.1.UNK</t>
+  </si>
+  <si>
+    <t>07262016.WKA.SU-30.3.1.UNK-A</t>
+  </si>
+  <si>
+    <t>07262016.WKA.SU-01.15.UNK</t>
+  </si>
+  <si>
+    <t>07262016.WKA.SU-01.15.UNK-A</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -527,12 +529,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,7 +1134,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>4.7600000000000003E-2</v>
@@ -1152,7 +1154,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>2.7300000000000001E-2</v>
@@ -1172,7 +1174,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>3.3599999999999998E-2</v>
@@ -1192,7 +1194,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <v>1.52E-2</v>
@@ -1212,7 +1214,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>3.0099999999999998E-2</v>
@@ -1232,7 +1234,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <v>2.46E-2</v>
@@ -1252,7 +1254,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B42">
         <v>0.15959999999999999</v>
@@ -1272,7 +1274,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B43">
         <v>7.6799999999999993E-2</v>

</xml_diff>